<commit_message>
Fix: Change 'count' column creatation for unique device_names
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1143,10 +1143,10 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>359</v>
+        <v>1499.98</v>
       </c>
       <c r="C2">
-        <v>2169</v>
+        <v>36378</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1160,10 +1160,10 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>10.01</v>
+        <v>584.96</v>
       </c>
       <c r="C3">
-        <v>9122</v>
+        <v>18707</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1177,10 +1177,10 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>174.03</v>
+        <v>1356.04</v>
       </c>
       <c r="C4">
-        <v>2193</v>
+        <v>20882</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1194,10 +1194,10 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>14.44</v>
+        <v>393.28</v>
       </c>
       <c r="C5">
-        <v>5153</v>
+        <v>14810</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1228,10 +1228,10 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>71.08</v>
+        <v>252.36</v>
       </c>
       <c r="C7">
-        <v>2006</v>
+        <v>8017</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1245,10 +1245,10 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>232.2</v>
+        <v>505.87</v>
       </c>
       <c r="C8">
-        <v>4137</v>
+        <v>9770</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1262,16 +1262,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>39.92</v>
+        <v>2953.76</v>
       </c>
       <c r="C9">
-        <v>9297</v>
+        <v>88596</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>86.86999999999999</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1279,13 +1279,13 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>8.699999999999999</v>
+        <v>969.77</v>
       </c>
       <c r="C10">
-        <v>5714</v>
+        <v>10167</v>
       </c>
       <c r="D10">
-        <v>0.48</v>
+        <v>53.87</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1296,10 +1296,10 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>136.19</v>
+        <v>567.75</v>
       </c>
       <c r="C11">
-        <v>7842</v>
+        <v>36344</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1313,10 +1313,10 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>250</v>
+        <v>1847.64</v>
       </c>
       <c r="C12">
-        <v>1851</v>
+        <v>30696</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -1330,13 +1330,13 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>271.12</v>
+        <v>277.5</v>
       </c>
       <c r="C13">
-        <v>3405</v>
+        <v>9911</v>
       </c>
       <c r="D13">
-        <v>38.73</v>
+        <v>39.63999999999999</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1347,10 +1347,10 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>172.78</v>
+        <v>466.71</v>
       </c>
       <c r="C14">
-        <v>5407</v>
+        <v>12851</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1364,10 +1364,10 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>354.05</v>
+        <v>1688.85</v>
       </c>
       <c r="C15">
-        <v>4905</v>
+        <v>30430</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1381,10 +1381,10 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>820.6600000000001</v>
       </c>
       <c r="C16">
-        <v>3515</v>
+        <v>15744</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1398,13 +1398,13 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>654.4299999999999</v>
+        <v>2139.1</v>
       </c>
       <c r="C17">
-        <v>4718</v>
+        <v>23898</v>
       </c>
       <c r="D17">
-        <v>40.9</v>
+        <v>133.7</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1415,16 +1415,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>144.69</v>
+        <v>3130.62</v>
       </c>
       <c r="C18">
-        <v>6139</v>
+        <v>63236</v>
       </c>
       <c r="D18">
-        <v>10.34</v>
+        <v>111.81</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1432,10 +1432,10 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.33</v>
+        <v>546.97</v>
       </c>
       <c r="C19">
-        <v>7268</v>
+        <v>15624</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1449,10 +1449,10 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>57.23</v>
+        <v>66.91</v>
       </c>
       <c r="C20">
-        <v>6650</v>
+        <v>10314</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1466,10 +1466,10 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>839.1799999999999</v>
+        <v>985.55</v>
       </c>
       <c r="C21">
-        <v>5922</v>
+        <v>12755</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1483,13 +1483,13 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>595.4299999999999</v>
+        <v>1542.49</v>
       </c>
       <c r="C22">
-        <v>1431</v>
+        <v>38432</v>
       </c>
       <c r="D22">
-        <v>66.16</v>
+        <v>171.38</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1500,10 +1500,10 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>575.59</v>
+        <v>1923.25</v>
       </c>
       <c r="C23">
-        <v>9618</v>
+        <v>41848</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1517,13 +1517,13 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>831.9</v>
+        <v>1300.14</v>
       </c>
       <c r="C24">
-        <v>7356</v>
+        <v>15134</v>
       </c>
       <c r="D24">
-        <v>138.65</v>
+        <v>216.69</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1534,13 +1534,13 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>90.94</v>
+        <v>1567.92</v>
       </c>
       <c r="C25">
-        <v>9969</v>
+        <v>46761</v>
       </c>
       <c r="D25">
-        <v>5.68</v>
+        <v>98.00000000000003</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1551,16 +1551,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>134.8</v>
+        <v>3041.56</v>
       </c>
       <c r="C26">
-        <v>5285</v>
+        <v>83300</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>760.4</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1568,10 +1568,10 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>663.27</v>
+        <v>755.73</v>
       </c>
       <c r="C27">
-        <v>3818</v>
+        <v>20997</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1602,10 +1602,10 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>77.67</v>
+        <v>726.9</v>
       </c>
       <c r="C29">
-        <v>1681</v>
+        <v>27250</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1619,10 +1619,10 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>484.98</v>
+        <v>1370.94</v>
       </c>
       <c r="C30">
-        <v>9224</v>
+        <v>22575</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1636,10 +1636,10 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>116.89</v>
+        <v>663.92</v>
       </c>
       <c r="C31">
-        <v>3488</v>
+        <v>15074</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1653,13 +1653,13 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>189.67</v>
+        <v>1142.71</v>
       </c>
       <c r="C32">
-        <v>5555</v>
+        <v>30804</v>
       </c>
       <c r="D32">
-        <v>31.61</v>
+        <v>190.45</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1670,10 +1670,10 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>42.74</v>
+        <v>189.36</v>
       </c>
       <c r="C33">
-        <v>6082</v>
+        <v>21878</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1687,13 +1687,13 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>76.13</v>
+        <v>549.6</v>
       </c>
       <c r="C34">
-        <v>2139</v>
+        <v>12630</v>
       </c>
       <c r="D34">
-        <v>5.86</v>
+        <v>42.28</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1704,16 +1704,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>52.39</v>
+        <v>4347.94</v>
       </c>
       <c r="C35">
-        <v>4059</v>
+        <v>92536</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1721,10 +1721,10 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>366.52</v>
+        <v>1405.76</v>
       </c>
       <c r="C36">
-        <v>8658</v>
+        <v>61937</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1738,10 +1738,10 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>65.17</v>
+        <v>1199.31</v>
       </c>
       <c r="C37">
-        <v>7817</v>
+        <v>32117</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1755,13 +1755,13 @@
         <v>41</v>
       </c>
       <c r="B38">
-        <v>70.78</v>
+        <v>97.04000000000001</v>
       </c>
       <c r="C38">
-        <v>4921</v>
+        <v>14238</v>
       </c>
       <c r="D38">
-        <v>4.16</v>
+        <v>5.7</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1789,10 +1789,10 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>89.95</v>
+        <v>1165.02</v>
       </c>
       <c r="C40">
-        <v>5224</v>
+        <v>22856</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1806,10 +1806,10 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>272.71</v>
+        <v>586.88</v>
       </c>
       <c r="C41">
-        <v>8347</v>
+        <v>12325</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1823,10 +1823,10 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>602.35</v>
+        <v>1620.88</v>
       </c>
       <c r="C42">
-        <v>7911</v>
+        <v>18490</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1840,10 +1840,10 @@
         <v>46</v>
       </c>
       <c r="B43">
-        <v>225.44</v>
+        <v>1185.21</v>
       </c>
       <c r="C43">
-        <v>4729</v>
+        <v>39439</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1857,13 +1857,13 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>617.97</v>
+        <v>1943.95</v>
       </c>
       <c r="C44">
-        <v>9550</v>
+        <v>47741</v>
       </c>
       <c r="D44">
-        <v>47.54</v>
+        <v>149.53</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1874,13 +1874,13 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>469.93</v>
+        <v>1031.24</v>
       </c>
       <c r="C45">
-        <v>1818</v>
+        <v>15496</v>
       </c>
       <c r="D45">
-        <v>156.64</v>
+        <v>343.74</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1891,10 +1891,10 @@
         <v>49</v>
       </c>
       <c r="B46">
-        <v>708.38</v>
+        <v>2316.77</v>
       </c>
       <c r="C46">
-        <v>5375</v>
+        <v>28208</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1908,10 +1908,10 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <v>456.25</v>
+        <v>973.2</v>
       </c>
       <c r="C47">
-        <v>9873</v>
+        <v>25842</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1925,13 +1925,13 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>197.27</v>
+        <v>432.67</v>
       </c>
       <c r="C48">
-        <v>7165</v>
+        <v>19597</v>
       </c>
       <c r="D48">
-        <v>49.32</v>
+        <v>108.17</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1942,10 +1942,10 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>203.22</v>
+        <v>782.47</v>
       </c>
       <c r="C49">
-        <v>5664</v>
+        <v>23772</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1959,10 +1959,10 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>301.49</v>
+        <v>1147.26</v>
       </c>
       <c r="C50">
-        <v>7497</v>
+        <v>27432</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1976,13 +1976,13 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>215.64</v>
+        <v>278.1</v>
       </c>
       <c r="C51">
-        <v>5666</v>
+        <v>11985</v>
       </c>
       <c r="D51">
-        <v>10.78</v>
+        <v>13.9</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1993,10 +1993,10 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>229.87</v>
+        <v>1059.55</v>
       </c>
       <c r="C52">
-        <v>5838</v>
+        <v>19084</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2010,16 +2010,16 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>218.98</v>
+        <v>3805.360000000001</v>
       </c>
       <c r="C53">
-        <v>1928</v>
+        <v>109504</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2027,13 +2027,13 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>402.53</v>
+        <v>781.02</v>
       </c>
       <c r="C54">
-        <v>3632</v>
+        <v>12963</v>
       </c>
       <c r="D54">
-        <v>40.25</v>
+        <v>78.09999999999999</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2044,10 +2044,10 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>130.08</v>
+        <v>705.17</v>
       </c>
       <c r="C55">
-        <v>6536</v>
+        <v>22826</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -2061,10 +2061,10 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>97.59</v>
+        <v>244.42</v>
       </c>
       <c r="C56">
-        <v>6671</v>
+        <v>11835</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -2078,10 +2078,10 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>349.01</v>
+        <v>1114.69</v>
       </c>
       <c r="C57">
-        <v>6806</v>
+        <v>46447</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -2095,13 +2095,13 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>260.34</v>
+        <v>739.46</v>
       </c>
       <c r="C58">
-        <v>1302</v>
+        <v>15362</v>
       </c>
       <c r="D58">
-        <v>20.03</v>
+        <v>56.89</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2112,10 +2112,10 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>14.14</v>
+        <v>340.93</v>
       </c>
       <c r="C59">
-        <v>6957</v>
+        <v>8739</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -2129,10 +2129,10 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>581.24</v>
+        <v>1954.62</v>
       </c>
       <c r="C60">
-        <v>6947</v>
+        <v>29756</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -2146,10 +2146,10 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>466.27</v>
+        <v>1364.32</v>
       </c>
       <c r="C61">
-        <v>2436</v>
+        <v>31967</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -2163,16 +2163,16 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>12.75</v>
+        <v>2930</v>
       </c>
       <c r="C62">
-        <v>4957</v>
+        <v>58462</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>488.34</v>
       </c>
       <c r="E62">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2180,10 +2180,10 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>66.72</v>
+        <v>579.36</v>
       </c>
       <c r="C63">
-        <v>5825</v>
+        <v>19759</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -2197,10 +2197,10 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>94.08</v>
+        <v>606.63</v>
       </c>
       <c r="C64">
-        <v>8629</v>
+        <v>28589</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2214,10 +2214,10 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>413.33</v>
+        <v>586.02</v>
       </c>
       <c r="C65">
-        <v>3634</v>
+        <v>12116</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2231,13 +2231,13 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>185.21</v>
+        <v>1378.57</v>
       </c>
       <c r="C66">
-        <v>5837</v>
+        <v>28607</v>
       </c>
       <c r="D66">
-        <v>30.87</v>
+        <v>229.77</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2248,10 +2248,10 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>40.92</v>
+        <v>707.9699999999999</v>
       </c>
       <c r="C67">
-        <v>2238</v>
+        <v>6706</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2265,13 +2265,13 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>238.01</v>
+        <v>1669.8</v>
       </c>
       <c r="C68">
-        <v>6213</v>
+        <v>40853</v>
       </c>
       <c r="D68">
-        <v>23.8</v>
+        <v>166.98</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -2282,10 +2282,10 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>145.73</v>
+        <v>334.37</v>
       </c>
       <c r="C69">
-        <v>7299</v>
+        <v>25612</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -2299,13 +2299,13 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>156.57</v>
+        <v>530.42</v>
       </c>
       <c r="C70">
-        <v>7633</v>
+        <v>19480</v>
       </c>
       <c r="D70">
-        <v>11.18</v>
+        <v>37.88</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2316,16 +2316,16 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>115.94</v>
+        <v>853.92</v>
       </c>
       <c r="C71">
-        <v>1489</v>
+        <v>19044</v>
       </c>
       <c r="D71">
-        <v>115.94</v>
+        <v>487.95</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2333,13 +2333,13 @@
         <v>75</v>
       </c>
       <c r="B72">
-        <v>391.7</v>
+        <v>1911.33</v>
       </c>
       <c r="C72">
-        <v>4387</v>
+        <v>24530</v>
       </c>
       <c r="D72">
-        <v>130.57</v>
+        <v>637.11</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2350,10 +2350,10 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>41.8</v>
+        <v>1299.18</v>
       </c>
       <c r="C73">
-        <v>4374</v>
+        <v>23463</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -2367,10 +2367,10 @@
         <v>77</v>
       </c>
       <c r="B74">
-        <v>217.83</v>
+        <v>1042.14</v>
       </c>
       <c r="C74">
-        <v>1031</v>
+        <v>19180</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -2384,10 +2384,10 @@
         <v>78</v>
       </c>
       <c r="B75">
-        <v>190.14</v>
+        <v>838.28</v>
       </c>
       <c r="C75">
-        <v>2748</v>
+        <v>20229</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -2401,10 +2401,10 @@
         <v>79</v>
       </c>
       <c r="B76">
-        <v>317.4</v>
+        <v>514.5599999999999</v>
       </c>
       <c r="C76">
-        <v>5945</v>
+        <v>18116</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -2418,13 +2418,13 @@
         <v>80</v>
       </c>
       <c r="B77">
-        <v>183.25</v>
+        <v>782.8299999999999</v>
       </c>
       <c r="C77">
-        <v>6414</v>
+        <v>16482</v>
       </c>
       <c r="D77">
-        <v>26.18</v>
+        <v>111.83</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -2435,10 +2435,10 @@
         <v>81</v>
       </c>
       <c r="B78">
-        <v>79.72</v>
+        <v>1234.8</v>
       </c>
       <c r="C78">
-        <v>4695</v>
+        <v>21536</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -2452,16 +2452,16 @@
         <v>82</v>
       </c>
       <c r="B79">
-        <v>80.68000000000001</v>
+        <v>2740.88</v>
       </c>
       <c r="C79">
-        <v>3448</v>
+        <v>65668</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>72.14</v>
       </c>
       <c r="E79">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2469,13 +2469,13 @@
         <v>83</v>
       </c>
       <c r="B80">
-        <v>187.14</v>
+        <v>1391.15</v>
       </c>
       <c r="C80">
-        <v>7752</v>
+        <v>34459</v>
       </c>
       <c r="D80">
-        <v>12.48</v>
+        <v>92.75</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -2486,10 +2486,10 @@
         <v>84</v>
       </c>
       <c r="B81">
-        <v>461</v>
+        <v>920.4599999999999</v>
       </c>
       <c r="C81">
-        <v>2768</v>
+        <v>20660</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2520,10 +2520,10 @@
         <v>86</v>
       </c>
       <c r="B83">
-        <v>3.36</v>
+        <v>2192.53</v>
       </c>
       <c r="C83">
-        <v>2738</v>
+        <v>29634</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -2537,10 +2537,10 @@
         <v>87</v>
       </c>
       <c r="B84">
-        <v>79.14</v>
+        <v>569.6</v>
       </c>
       <c r="C84">
-        <v>6885</v>
+        <v>28840</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -2571,13 +2571,13 @@
         <v>89</v>
       </c>
       <c r="B86">
-        <v>97.5</v>
+        <v>310.0600000000001</v>
       </c>
       <c r="C86">
-        <v>4159</v>
+        <v>24892</v>
       </c>
       <c r="D86">
-        <v>5.74</v>
+        <v>18.24</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -2588,10 +2588,10 @@
         <v>90</v>
       </c>
       <c r="B87">
-        <v>87.06</v>
+        <v>1193.78</v>
       </c>
       <c r="C87">
-        <v>8539</v>
+        <v>33068</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -2605,16 +2605,16 @@
         <v>91</v>
       </c>
       <c r="B88">
-        <v>306.71</v>
+        <v>3837.42</v>
       </c>
       <c r="C88">
-        <v>2000</v>
+        <v>51140</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2622,10 +2622,10 @@
         <v>92</v>
       </c>
       <c r="B89">
-        <v>159.81</v>
+        <v>625</v>
       </c>
       <c r="C89">
-        <v>3463</v>
+        <v>27442</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -2639,10 +2639,10 @@
         <v>93</v>
       </c>
       <c r="B90">
-        <v>71.95999999999999</v>
+        <v>1112.77</v>
       </c>
       <c r="C90">
-        <v>9987</v>
+        <v>31130</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -2656,10 +2656,10 @@
         <v>94</v>
       </c>
       <c r="B91">
-        <v>4.61</v>
+        <v>668.0599999999999</v>
       </c>
       <c r="C91">
-        <v>5399</v>
+        <v>16288</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -2673,13 +2673,13 @@
         <v>95</v>
       </c>
       <c r="B92">
-        <v>540.54</v>
+        <v>1627.88</v>
       </c>
       <c r="C92">
-        <v>5018</v>
+        <v>38029</v>
       </c>
       <c r="D92">
-        <v>108.11</v>
+        <v>325.58</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -2690,10 +2690,10 @@
         <v>96</v>
       </c>
       <c r="B93">
-        <v>43.85</v>
+        <v>1358.62</v>
       </c>
       <c r="C93">
-        <v>6891</v>
+        <v>31056</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -2707,10 +2707,10 @@
         <v>97</v>
       </c>
       <c r="B94">
-        <v>165.77</v>
+        <v>1086.94</v>
       </c>
       <c r="C94">
-        <v>6532</v>
+        <v>28941</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -2724,10 +2724,10 @@
         <v>98</v>
       </c>
       <c r="B95">
-        <v>495.71</v>
+        <v>572.9299999999999</v>
       </c>
       <c r="C95">
-        <v>2513</v>
+        <v>5959</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2741,10 +2741,10 @@
         <v>99</v>
       </c>
       <c r="B96">
-        <v>56.05</v>
+        <v>400.09</v>
       </c>
       <c r="C96">
-        <v>4520</v>
+        <v>19554</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2758,16 +2758,16 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>282.78</v>
+        <v>5285.139999999999</v>
       </c>
       <c r="C97">
-        <v>8842</v>
+        <v>93508</v>
       </c>
       <c r="D97">
         <v>0</v>
       </c>
       <c r="E97">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2775,10 +2775,10 @@
         <v>101</v>
       </c>
       <c r="B98">
-        <v>182.51</v>
+        <v>881.09</v>
       </c>
       <c r="C98">
-        <v>8066</v>
+        <v>16595</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -2792,13 +2792,13 @@
         <v>102</v>
       </c>
       <c r="B99">
-        <v>261.88</v>
+        <v>1176.68</v>
       </c>
       <c r="C99">
-        <v>3735</v>
+        <v>18234</v>
       </c>
       <c r="D99">
-        <v>15.4</v>
+        <v>69.20999999999999</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -2809,10 +2809,10 @@
         <v>103</v>
       </c>
       <c r="B100">
-        <v>122.44</v>
+        <v>1224.57</v>
       </c>
       <c r="C100">
-        <v>6946</v>
+        <v>29503</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -2826,13 +2826,13 @@
         <v>104</v>
       </c>
       <c r="B101">
-        <v>415.67</v>
+        <v>1411.91</v>
       </c>
       <c r="C101">
-        <v>1404</v>
+        <v>16622</v>
       </c>
       <c r="D101">
-        <v>207.84</v>
+        <v>705.97</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -2843,13 +2843,13 @@
         <v>105</v>
       </c>
       <c r="B102">
-        <v>56.29</v>
+        <v>682.9400000000001</v>
       </c>
       <c r="C102">
-        <v>3337</v>
+        <v>18556</v>
       </c>
       <c r="D102">
-        <v>3.31</v>
+        <v>40.17</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -2860,10 +2860,10 @@
         <v>106</v>
       </c>
       <c r="B103">
-        <v>22.77</v>
+        <v>393.6199999999999</v>
       </c>
       <c r="C103">
-        <v>2283</v>
+        <v>9229</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -2877,10 +2877,10 @@
         <v>107</v>
       </c>
       <c r="B104">
-        <v>671.45</v>
+        <v>3200.54</v>
       </c>
       <c r="C104">
-        <v>1003</v>
+        <v>36427</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -2894,13 +2894,13 @@
         <v>108</v>
       </c>
       <c r="B105">
-        <v>368.7</v>
+        <v>1400.23</v>
       </c>
       <c r="C105">
-        <v>3404</v>
+        <v>42480</v>
       </c>
       <c r="D105">
-        <v>73.73999999999999</v>
+        <v>280.05</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -2911,16 +2911,16 @@
         <v>109</v>
       </c>
       <c r="B106">
-        <v>110.39</v>
+        <v>1612.26</v>
       </c>
       <c r="C106">
-        <v>2754</v>
+        <v>40098</v>
       </c>
       <c r="D106">
         <v>0</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2928,10 +2928,10 @@
         <v>110</v>
       </c>
       <c r="B107">
-        <v>41.43</v>
+        <v>1079.39</v>
       </c>
       <c r="C107">
-        <v>3480</v>
+        <v>28096</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -2945,10 +2945,10 @@
         <v>111</v>
       </c>
       <c r="B108">
-        <v>164.55</v>
+        <v>564.5</v>
       </c>
       <c r="C108">
-        <v>2993</v>
+        <v>12142</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -2962,10 +2962,10 @@
         <v>112</v>
       </c>
       <c r="B109">
-        <v>212.53</v>
+        <v>1462.45</v>
       </c>
       <c r="C109">
-        <v>5033</v>
+        <v>21601</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -2979,13 +2979,13 @@
         <v>113</v>
       </c>
       <c r="B110">
-        <v>133</v>
+        <v>415.35</v>
       </c>
       <c r="C110">
-        <v>2908</v>
+        <v>7522</v>
       </c>
       <c r="D110">
-        <v>14.78</v>
+        <v>46.15</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -2996,10 +2996,10 @@
         <v>114</v>
       </c>
       <c r="B111">
-        <v>44.54</v>
+        <v>2841.24</v>
       </c>
       <c r="C111">
-        <v>7844</v>
+        <v>48097</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -3030,10 +3030,10 @@
         <v>116</v>
       </c>
       <c r="B113">
-        <v>481.06</v>
+        <v>2451.12</v>
       </c>
       <c r="C113">
-        <v>9482</v>
+        <v>49836</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -3047,16 +3047,16 @@
         <v>117</v>
       </c>
       <c r="B114">
-        <v>959.53</v>
+        <v>5628.640000000001</v>
       </c>
       <c r="C114">
-        <v>1693</v>
+        <v>84482</v>
       </c>
       <c r="D114">
         <v>0</v>
       </c>
       <c r="E114">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3064,10 +3064,10 @@
         <v>118</v>
       </c>
       <c r="B115">
-        <v>553.3</v>
+        <v>1278.55</v>
       </c>
       <c r="C115">
-        <v>1584</v>
+        <v>20161</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -3081,10 +3081,10 @@
         <v>119</v>
       </c>
       <c r="B116">
-        <v>339.98</v>
+        <v>1924.81</v>
       </c>
       <c r="C116">
-        <v>5837</v>
+        <v>33450</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -3098,13 +3098,13 @@
         <v>120</v>
       </c>
       <c r="B117">
-        <v>288.13</v>
+        <v>1626.73</v>
       </c>
       <c r="C117">
-        <v>2694</v>
+        <v>29165</v>
       </c>
       <c r="D117">
-        <v>36.02</v>
+        <v>203.34</v>
       </c>
       <c r="E117">
         <v>1</v>
@@ -3115,10 +3115,10 @@
         <v>121</v>
       </c>
       <c r="B118">
-        <v>549.3099999999999</v>
+        <v>1384.83</v>
       </c>
       <c r="C118">
-        <v>4847</v>
+        <v>16666</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -3132,10 +3132,10 @@
         <v>122</v>
       </c>
       <c r="B119">
-        <v>360.85</v>
+        <v>1967.93</v>
       </c>
       <c r="C119">
-        <v>4629</v>
+        <v>22073</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -3149,13 +3149,13 @@
         <v>123</v>
       </c>
       <c r="B120">
-        <v>36.99</v>
+        <v>454.03</v>
       </c>
       <c r="C120">
-        <v>1446</v>
+        <v>11646</v>
       </c>
       <c r="D120">
-        <v>1.95</v>
+        <v>23.9</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -3166,10 +3166,10 @@
         <v>124</v>
       </c>
       <c r="B121">
-        <v>278.78</v>
+        <v>961.5599999999999</v>
       </c>
       <c r="C121">
-        <v>5026</v>
+        <v>21620</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -3183,16 +3183,16 @@
         <v>125</v>
       </c>
       <c r="B122">
-        <v>2.9</v>
+        <v>1472.62</v>
       </c>
       <c r="C122">
-        <v>9427</v>
+        <v>93760</v>
       </c>
       <c r="D122">
-        <v>0.41</v>
+        <v>105.19</v>
       </c>
       <c r="E122">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3200,10 +3200,10 @@
         <v>126</v>
       </c>
       <c r="B123">
-        <v>224.9</v>
+        <v>606.38</v>
       </c>
       <c r="C123">
-        <v>6957</v>
+        <v>11444</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -3217,10 +3217,10 @@
         <v>127</v>
       </c>
       <c r="B124">
-        <v>313.86</v>
+        <v>1216.02</v>
       </c>
       <c r="C124">
-        <v>3031</v>
+        <v>18282</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -3234,10 +3234,10 @@
         <v>128</v>
       </c>
       <c r="B125">
-        <v>519</v>
+        <v>995.0300000000001</v>
       </c>
       <c r="C125">
-        <v>5423</v>
+        <v>31999</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -3268,10 +3268,10 @@
         <v>130</v>
       </c>
       <c r="B127">
-        <v>543.92</v>
+        <v>1916.88</v>
       </c>
       <c r="C127">
-        <v>1917</v>
+        <v>14565</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -3285,13 +3285,13 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>124.71</v>
+        <v>181.94</v>
       </c>
       <c r="C128">
-        <v>9143</v>
+        <v>38937</v>
       </c>
       <c r="D128">
-        <v>6.93</v>
+        <v>10.11</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -3302,10 +3302,10 @@
         <v>132</v>
       </c>
       <c r="B129">
-        <v>31.74</v>
+        <v>326.44</v>
       </c>
       <c r="C129">
-        <v>4582</v>
+        <v>13617</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -3319,10 +3319,10 @@
         <v>133</v>
       </c>
       <c r="B130">
-        <v>30.05</v>
+        <v>670.0999999999999</v>
       </c>
       <c r="C130">
-        <v>5145</v>
+        <v>15197</v>
       </c>
       <c r="D130">
         <v>0</v>
@@ -3336,16 +3336,16 @@
         <v>134</v>
       </c>
       <c r="B131">
-        <v>492.75</v>
+        <v>5737.66</v>
       </c>
       <c r="C131">
-        <v>2228</v>
+        <v>55172</v>
       </c>
       <c r="D131">
         <v>0</v>
       </c>
       <c r="E131">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3353,10 +3353,10 @@
         <v>135</v>
       </c>
       <c r="B132">
-        <v>326.83</v>
+        <v>1416.75</v>
       </c>
       <c r="C132">
-        <v>6496</v>
+        <v>35067</v>
       </c>
       <c r="D132">
         <v>0</v>
@@ -3370,10 +3370,10 @@
         <v>136</v>
       </c>
       <c r="B133">
-        <v>79.98999999999999</v>
+        <v>1113.33</v>
       </c>
       <c r="C133">
-        <v>5524</v>
+        <v>46385</v>
       </c>
       <c r="D133">
         <v>0</v>
@@ -3404,10 +3404,10 @@
         <v>138</v>
       </c>
       <c r="B135">
-        <v>796.15</v>
+        <v>1672.78</v>
       </c>
       <c r="C135">
-        <v>5521</v>
+        <v>12635</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -3421,10 +3421,10 @@
         <v>139</v>
       </c>
       <c r="B136">
-        <v>31.11</v>
+        <v>933.5599999999999</v>
       </c>
       <c r="C136">
-        <v>6720</v>
+        <v>37542</v>
       </c>
       <c r="D136">
         <v>0</v>
@@ -3438,10 +3438,10 @@
         <v>140</v>
       </c>
       <c r="B137">
-        <v>322.47</v>
+        <v>1646.81</v>
       </c>
       <c r="C137">
-        <v>3556</v>
+        <v>30663</v>
       </c>
       <c r="D137">
         <v>0</v>
@@ -3455,10 +3455,10 @@
         <v>141</v>
       </c>
       <c r="B138">
-        <v>65.63</v>
+        <v>1245.16</v>
       </c>
       <c r="C138">
-        <v>4421</v>
+        <v>17252</v>
       </c>
       <c r="D138">
         <v>0</v>
@@ -3472,10 +3472,10 @@
         <v>142</v>
       </c>
       <c r="B139">
-        <v>105.53</v>
+        <v>840.14</v>
       </c>
       <c r="C139">
-        <v>4062</v>
+        <v>36080</v>
       </c>
       <c r="D139">
         <v>0</v>
@@ -3489,16 +3489,16 @@
         <v>143</v>
       </c>
       <c r="B140">
-        <v>520.74</v>
+        <v>4899.719999999999</v>
       </c>
       <c r="C140">
-        <v>1665</v>
+        <v>92446</v>
       </c>
       <c r="D140">
-        <v>65.09</v>
+        <v>306.22</v>
       </c>
       <c r="E140">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3506,10 +3506,10 @@
         <v>144</v>
       </c>
       <c r="B141">
-        <v>563.26</v>
+        <v>948.0400000000001</v>
       </c>
       <c r="C141">
-        <v>1166</v>
+        <v>6997</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -3523,10 +3523,10 @@
         <v>145</v>
       </c>
       <c r="B142">
-        <v>147.19</v>
+        <v>1828.31</v>
       </c>
       <c r="C142">
-        <v>1259</v>
+        <v>19388</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -3540,10 +3540,10 @@
         <v>146</v>
       </c>
       <c r="B143">
-        <v>24.05</v>
+        <v>312.1</v>
       </c>
       <c r="C143">
-        <v>3354</v>
+        <v>26648</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -3557,10 +3557,10 @@
         <v>147</v>
       </c>
       <c r="B144">
-        <v>496.82</v>
+        <v>873.01</v>
       </c>
       <c r="C144">
-        <v>3047</v>
+        <v>5717</v>
       </c>
       <c r="D144">
         <v>0</v>
@@ -3574,10 +3574,10 @@
         <v>148</v>
       </c>
       <c r="B145">
-        <v>538.9400000000001</v>
+        <v>1001.2</v>
       </c>
       <c r="C145">
-        <v>8651</v>
+        <v>44735</v>
       </c>
       <c r="D145">
         <v>0</v>
@@ -3608,10 +3608,10 @@
         <v>150</v>
       </c>
       <c r="B147">
-        <v>8.59</v>
+        <v>160.54</v>
       </c>
       <c r="C147">
-        <v>6487</v>
+        <v>24300</v>
       </c>
       <c r="D147">
         <v>0</v>
@@ -3625,13 +3625,13 @@
         <v>151</v>
       </c>
       <c r="B148">
-        <v>48.51</v>
+        <v>780.15</v>
       </c>
       <c r="C148">
-        <v>8211</v>
+        <v>27408</v>
       </c>
       <c r="D148">
-        <v>2.55</v>
+        <v>41.05</v>
       </c>
       <c r="E148">
         <v>1</v>
@@ -3642,16 +3642,16 @@
         <v>152</v>
       </c>
       <c r="B149">
-        <v>22.96</v>
+        <v>2043</v>
       </c>
       <c r="C149">
-        <v>2370</v>
+        <v>35048</v>
       </c>
       <c r="D149">
         <v>0</v>
       </c>
       <c r="E149">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3659,10 +3659,10 @@
         <v>153</v>
       </c>
       <c r="B150">
-        <v>81.62</v>
+        <v>729.9599999999999</v>
       </c>
       <c r="C150">
-        <v>9603</v>
+        <v>27639</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -3676,10 +3676,10 @@
         <v>154</v>
       </c>
       <c r="B151">
-        <v>28.47</v>
+        <v>275.23</v>
       </c>
       <c r="C151">
-        <v>4562</v>
+        <v>12366</v>
       </c>
       <c r="D151">
         <v>0</v>
@@ -3693,10 +3693,10 @@
         <v>155</v>
       </c>
       <c r="B152">
-        <v>363.66</v>
+        <v>758.5300000000001</v>
       </c>
       <c r="C152">
-        <v>3211</v>
+        <v>20327</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -3727,10 +3727,10 @@
         <v>157</v>
       </c>
       <c r="B154">
-        <v>663.6799999999999</v>
+        <v>1238.65</v>
       </c>
       <c r="C154">
-        <v>6966</v>
+        <v>11126</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -3744,10 +3744,10 @@
         <v>158</v>
       </c>
       <c r="B155">
-        <v>96.31</v>
+        <v>991.79</v>
       </c>
       <c r="C155">
-        <v>1166</v>
+        <v>17424</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -3761,10 +3761,10 @@
         <v>159</v>
       </c>
       <c r="B156">
-        <v>54.91</v>
+        <v>1167.85</v>
       </c>
       <c r="C156">
-        <v>9737</v>
+        <v>19418</v>
       </c>
       <c r="D156">
         <v>0</v>
@@ -3778,10 +3778,10 @@
         <v>160</v>
       </c>
       <c r="B157">
-        <v>78.66</v>
+        <v>80.84999999999999</v>
       </c>
       <c r="C157">
-        <v>4599</v>
+        <v>9057</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -3795,16 +3795,16 @@
         <v>161</v>
       </c>
       <c r="B158">
-        <v>47.92</v>
+        <v>8492.6</v>
       </c>
       <c r="C158">
-        <v>9646</v>
+        <v>164652</v>
       </c>
       <c r="D158">
-        <v>0</v>
+        <v>386.04</v>
       </c>
       <c r="E158">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3812,10 +3812,10 @@
         <v>162</v>
       </c>
       <c r="B159">
-        <v>294.82</v>
+        <v>1261.87</v>
       </c>
       <c r="C159">
-        <v>9319</v>
+        <v>22824</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -3846,13 +3846,13 @@
         <v>164</v>
       </c>
       <c r="B161">
-        <v>99.58</v>
+        <v>612.78</v>
       </c>
       <c r="C161">
-        <v>3644</v>
+        <v>15298</v>
       </c>
       <c r="D161">
-        <v>11.06</v>
+        <v>68.09</v>
       </c>
       <c r="E161">
         <v>1</v>
@@ -3863,10 +3863,10 @@
         <v>165</v>
       </c>
       <c r="B162">
-        <v>95.81</v>
+        <v>411.9300000000001</v>
       </c>
       <c r="C162">
-        <v>6131</v>
+        <v>19990</v>
       </c>
       <c r="D162">
         <v>0</v>
@@ -3880,10 +3880,10 @@
         <v>166</v>
       </c>
       <c r="B163">
-        <v>484.81</v>
+        <v>2080.28</v>
       </c>
       <c r="C163">
-        <v>4895</v>
+        <v>44931</v>
       </c>
       <c r="D163">
         <v>0</v>
@@ -3897,13 +3897,13 @@
         <v>167</v>
       </c>
       <c r="B164">
-        <v>41.53</v>
+        <v>597.7800000000001</v>
       </c>
       <c r="C164">
-        <v>6901</v>
+        <v>27560</v>
       </c>
       <c r="D164">
-        <v>5.19</v>
+        <v>74.72999999999999</v>
       </c>
       <c r="E164">
         <v>1</v>
@@ -3914,10 +3914,10 @@
         <v>168</v>
       </c>
       <c r="B165">
-        <v>185.37</v>
+        <v>911.11</v>
       </c>
       <c r="C165">
-        <v>2252</v>
+        <v>14024</v>
       </c>
       <c r="D165">
         <v>0</v>
@@ -3931,10 +3931,10 @@
         <v>169</v>
       </c>
       <c r="B166">
-        <v>411.61</v>
+        <v>993.0599999999999</v>
       </c>
       <c r="C166">
-        <v>5496</v>
+        <v>16312</v>
       </c>
       <c r="D166">
         <v>0</v>
@@ -3948,16 +3948,16 @@
         <v>170</v>
       </c>
       <c r="B167">
-        <v>106.69</v>
+        <v>2473.96</v>
       </c>
       <c r="C167">
-        <v>2935</v>
+        <v>82524</v>
       </c>
       <c r="D167">
         <v>0</v>
       </c>
       <c r="E167">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3965,13 +3965,13 @@
         <v>171</v>
       </c>
       <c r="B168">
-        <v>13.15</v>
+        <v>95.09</v>
       </c>
       <c r="C168">
-        <v>7012</v>
+        <v>19072</v>
       </c>
       <c r="D168">
-        <v>0.77</v>
+        <v>5.59</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -3982,10 +3982,10 @@
         <v>172</v>
       </c>
       <c r="B169">
-        <v>53.17</v>
+        <v>1037.92</v>
       </c>
       <c r="C169">
-        <v>1722</v>
+        <v>14081</v>
       </c>
       <c r="D169">
         <v>0</v>
@@ -3999,10 +3999,10 @@
         <v>173</v>
       </c>
       <c r="B170">
-        <v>215.05</v>
+        <v>2216.49</v>
       </c>
       <c r="C170">
-        <v>4316</v>
+        <v>35725</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -4016,10 +4016,10 @@
         <v>174</v>
       </c>
       <c r="B171">
-        <v>862.3</v>
+        <v>884.63</v>
       </c>
       <c r="C171">
-        <v>5555</v>
+        <v>11969</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -4033,10 +4033,10 @@
         <v>175</v>
       </c>
       <c r="B172">
-        <v>89.63</v>
+        <v>386.44</v>
       </c>
       <c r="C172">
-        <v>3215</v>
+        <v>5354</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -4050,10 +4050,10 @@
         <v>176</v>
       </c>
       <c r="B173">
-        <v>299.03</v>
+        <v>622.5399999999998</v>
       </c>
       <c r="C173">
-        <v>3997</v>
+        <v>15900</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -4084,16 +4084,16 @@
         <v>178</v>
       </c>
       <c r="B175">
-        <v>288.65</v>
+        <v>5963.760000000001</v>
       </c>
       <c r="C175">
-        <v>8227</v>
+        <v>100430</v>
       </c>
       <c r="D175">
-        <v>28.86</v>
+        <v>298.18</v>
       </c>
       <c r="E175">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4101,10 +4101,10 @@
         <v>179</v>
       </c>
       <c r="B176">
-        <v>299.82</v>
+        <v>518.75</v>
       </c>
       <c r="C176">
-        <v>9083</v>
+        <v>23383</v>
       </c>
       <c r="D176">
         <v>0</v>
@@ -4135,10 +4135,10 @@
         <v>181</v>
       </c>
       <c r="B178">
-        <v>628.5</v>
+        <v>2282.05</v>
       </c>
       <c r="C178">
-        <v>8059</v>
+        <v>43617</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -4152,10 +4152,10 @@
         <v>182</v>
       </c>
       <c r="B179">
-        <v>28.93</v>
+        <v>44.13</v>
       </c>
       <c r="C179">
-        <v>4668</v>
+        <v>10672</v>
       </c>
       <c r="D179">
         <v>0</v>
@@ -4169,10 +4169,10 @@
         <v>183</v>
       </c>
       <c r="B180">
-        <v>232.69</v>
+        <v>1150.11</v>
       </c>
       <c r="C180">
-        <v>5594</v>
+        <v>16921</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -4186,10 +4186,10 @@
         <v>184</v>
       </c>
       <c r="B181">
-        <v>456.78</v>
+        <v>1319.46</v>
       </c>
       <c r="C181">
-        <v>1234</v>
+        <v>19455</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -4203,10 +4203,10 @@
         <v>185</v>
       </c>
       <c r="B182">
-        <v>44.54</v>
+        <v>1659.15</v>
       </c>
       <c r="C182">
-        <v>2866</v>
+        <v>37108</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -4220,10 +4220,10 @@
         <v>186</v>
       </c>
       <c r="B183">
-        <v>536.74</v>
+        <v>1674.9</v>
       </c>
       <c r="C183">
-        <v>1455</v>
+        <v>49598</v>
       </c>
       <c r="D183">
         <v>0</v>
@@ -4237,16 +4237,16 @@
         <v>187</v>
       </c>
       <c r="B184">
-        <v>787.22</v>
+        <v>7240.900000000003</v>
       </c>
       <c r="C184">
-        <v>9669</v>
+        <v>130208</v>
       </c>
       <c r="D184">
-        <v>52.48</v>
+        <v>241.37</v>
       </c>
       <c r="E184">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -4254,13 +4254,13 @@
         <v>188</v>
       </c>
       <c r="B185">
-        <v>21.16</v>
+        <v>920.7599999999999</v>
       </c>
       <c r="C185">
-        <v>7515</v>
+        <v>27121</v>
       </c>
       <c r="D185">
-        <v>5.29</v>
+        <v>230.18</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -4271,13 +4271,13 @@
         <v>189</v>
       </c>
       <c r="B186">
-        <v>31.31</v>
+        <v>1000.35</v>
       </c>
       <c r="C186">
-        <v>6106</v>
+        <v>26358</v>
       </c>
       <c r="D186">
-        <v>1.74</v>
+        <v>55.57</v>
       </c>
       <c r="E186">
         <v>1</v>
@@ -4288,10 +4288,10 @@
         <v>190</v>
       </c>
       <c r="B187">
-        <v>74.25</v>
+        <v>436.39</v>
       </c>
       <c r="C187">
-        <v>3896</v>
+        <v>12266</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -4305,10 +4305,10 @@
         <v>191</v>
       </c>
       <c r="B188">
-        <v>20.28</v>
+        <v>2007.77</v>
       </c>
       <c r="C188">
-        <v>3968</v>
+        <v>31493</v>
       </c>
       <c r="D188">
         <v>0</v>
@@ -4339,10 +4339,10 @@
         <v>193</v>
       </c>
       <c r="B190">
-        <v>213.94</v>
+        <v>1523.19</v>
       </c>
       <c r="C190">
-        <v>5687</v>
+        <v>38807</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -4356,13 +4356,13 @@
         <v>194</v>
       </c>
       <c r="B191">
-        <v>719.8099999999999</v>
+        <v>1302.93</v>
       </c>
       <c r="C191">
-        <v>8517</v>
+        <v>29219</v>
       </c>
       <c r="D191">
-        <v>59.98</v>
+        <v>108.57</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -4373,10 +4373,10 @@
         <v>195</v>
       </c>
       <c r="B192">
-        <v>114.36</v>
+        <v>1316.07</v>
       </c>
       <c r="C192">
-        <v>2989</v>
+        <v>46104</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -4390,16 +4390,16 @@
         <v>196</v>
       </c>
       <c r="B193">
-        <v>239.24</v>
+        <v>1685.22</v>
       </c>
       <c r="C193">
-        <v>6615</v>
+        <v>67042</v>
       </c>
       <c r="D193">
         <v>0</v>
       </c>
       <c r="E193">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -4407,10 +4407,10 @@
         <v>197</v>
       </c>
       <c r="B194">
-        <v>3.88</v>
+        <v>361.66</v>
       </c>
       <c r="C194">
-        <v>5261</v>
+        <v>17687</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -4424,10 +4424,10 @@
         <v>198</v>
       </c>
       <c r="B195">
-        <v>211.81</v>
+        <v>451.85</v>
       </c>
       <c r="C195">
-        <v>5578</v>
+        <v>13078</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -4441,10 +4441,10 @@
         <v>199</v>
       </c>
       <c r="B196">
-        <v>82.67</v>
+        <v>476.72</v>
       </c>
       <c r="C196">
-        <v>6838</v>
+        <v>19274</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -4458,10 +4458,10 @@
         <v>200</v>
       </c>
       <c r="B197">
-        <v>246.05</v>
+        <v>1812.85</v>
       </c>
       <c r="C197">
-        <v>8861</v>
+        <v>29438</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -4475,10 +4475,10 @@
         <v>201</v>
       </c>
       <c r="B198">
-        <v>40.56</v>
+        <v>1020.06</v>
       </c>
       <c r="C198">
-        <v>5379</v>
+        <v>32704</v>
       </c>
       <c r="D198">
         <v>0</v>
@@ -4492,10 +4492,10 @@
         <v>202</v>
       </c>
       <c r="B199">
-        <v>1.45</v>
+        <v>700.59</v>
       </c>
       <c r="C199">
-        <v>3991</v>
+        <v>16697</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -4509,10 +4509,10 @@
         <v>203</v>
       </c>
       <c r="B200">
-        <v>819.61</v>
+        <v>832.89</v>
       </c>
       <c r="C200">
-        <v>1137</v>
+        <v>5426</v>
       </c>
       <c r="D200">
         <v>0</v>
@@ -4526,10 +4526,10 @@
         <v>204</v>
       </c>
       <c r="B201">
-        <v>222.22</v>
+        <v>326.87</v>
       </c>
       <c r="C201">
-        <v>5541</v>
+        <v>13213</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -4543,16 +4543,16 @@
         <v>205</v>
       </c>
       <c r="B202">
-        <v>516.5599999999999</v>
+        <v>4456.719999999999</v>
       </c>
       <c r="C202">
-        <v>4032</v>
+        <v>120860</v>
       </c>
       <c r="D202">
-        <v>103.31</v>
+        <v>445.67</v>
       </c>
       <c r="E202">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4560,10 +4560,10 @@
         <v>206</v>
       </c>
       <c r="B203">
-        <v>427.83</v>
+        <v>1646.41</v>
       </c>
       <c r="C203">
-        <v>1549</v>
+        <v>33387</v>
       </c>
       <c r="D203">
         <v>0</v>
@@ -4577,10 +4577,10 @@
         <v>207</v>
       </c>
       <c r="B204">
-        <v>125.29</v>
+        <v>1668.64</v>
       </c>
       <c r="C204">
-        <v>2419</v>
+        <v>40972</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -4594,10 +4594,10 @@
         <v>208</v>
       </c>
       <c r="B205">
-        <v>165.73</v>
+        <v>347.4</v>
       </c>
       <c r="C205">
-        <v>9527</v>
+        <v>18303</v>
       </c>
       <c r="D205">
         <v>0</v>
@@ -4611,10 +4611,10 @@
         <v>209</v>
       </c>
       <c r="B206">
-        <v>87.14</v>
+        <v>1466.7</v>
       </c>
       <c r="C206">
-        <v>7081</v>
+        <v>40583</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -4628,10 +4628,10 @@
         <v>210</v>
       </c>
       <c r="B207">
-        <v>165.62</v>
+        <v>1531.92</v>
       </c>
       <c r="C207">
-        <v>5640</v>
+        <v>50838</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -4645,10 +4645,10 @@
         <v>211</v>
       </c>
       <c r="B208">
-        <v>568.4400000000001</v>
+        <v>1276.54</v>
       </c>
       <c r="C208">
-        <v>8375</v>
+        <v>21482</v>
       </c>
       <c r="D208">
         <v>0</v>
@@ -4662,13 +4662,13 @@
         <v>212</v>
       </c>
       <c r="B209">
-        <v>213.13</v>
+        <v>846.9199999999998</v>
       </c>
       <c r="C209">
-        <v>1333</v>
+        <v>17070</v>
       </c>
       <c r="D209">
-        <v>23.68</v>
+        <v>94.11</v>
       </c>
       <c r="E209">
         <v>1</v>
@@ -4679,10 +4679,10 @@
         <v>213</v>
       </c>
       <c r="B210">
-        <v>208.49</v>
+        <v>2632.67</v>
       </c>
       <c r="C210">
-        <v>7994</v>
+        <v>26638</v>
       </c>
       <c r="D210">
         <v>0</v>
@@ -4696,16 +4696,16 @@
         <v>214</v>
       </c>
       <c r="B211">
-        <v>49.12</v>
+        <v>4724.18</v>
       </c>
       <c r="C211">
-        <v>9344</v>
+        <v>79666</v>
       </c>
       <c r="D211">
         <v>0</v>
       </c>
       <c r="E211">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -4713,13 +4713,13 @@
         <v>215</v>
       </c>
       <c r="B212">
-        <v>105.57</v>
+        <v>687.8199999999999</v>
       </c>
       <c r="C212">
-        <v>2184</v>
+        <v>9580</v>
       </c>
       <c r="D212">
-        <v>5.56</v>
+        <v>36.2</v>
       </c>
       <c r="E212">
         <v>1</v>
@@ -4730,10 +4730,10 @@
         <v>216</v>
       </c>
       <c r="B213">
-        <v>103.27</v>
+        <v>1121.35</v>
       </c>
       <c r="C213">
-        <v>5186</v>
+        <v>34853</v>
       </c>
       <c r="D213">
         <v>0</v>
@@ -4747,10 +4747,10 @@
         <v>217</v>
       </c>
       <c r="B214">
-        <v>655.8099999999999</v>
+        <v>1562.47</v>
       </c>
       <c r="C214">
-        <v>9582</v>
+        <v>25182</v>
       </c>
       <c r="D214">
         <v>0</v>
@@ -4764,10 +4764,10 @@
         <v>218</v>
       </c>
       <c r="B215">
-        <v>2.5</v>
+        <v>657.47</v>
       </c>
       <c r="C215">
-        <v>3591</v>
+        <v>19086</v>
       </c>
       <c r="D215">
         <v>0</v>
@@ -4781,10 +4781,10 @@
         <v>219</v>
       </c>
       <c r="B216">
-        <v>146.54</v>
+        <v>1205.95</v>
       </c>
       <c r="C216">
-        <v>5997</v>
+        <v>28672</v>
       </c>
       <c r="D216">
         <v>0</v>
@@ -4798,10 +4798,10 @@
         <v>220</v>
       </c>
       <c r="B217">
-        <v>30.02</v>
+        <v>357.83</v>
       </c>
       <c r="C217">
-        <v>4135</v>
+        <v>15427</v>
       </c>
       <c r="D217">
         <v>0</v>
@@ -4815,13 +4815,13 @@
         <v>221</v>
       </c>
       <c r="B218">
-        <v>260.53</v>
+        <v>1219.34</v>
       </c>
       <c r="C218">
-        <v>4404</v>
+        <v>31742</v>
       </c>
       <c r="D218">
-        <v>21.71</v>
+        <v>101.62</v>
       </c>
       <c r="E218">
         <v>1</v>
@@ -4832,10 +4832,10 @@
         <v>222</v>
       </c>
       <c r="B219">
-        <v>79.18000000000001</v>
+        <v>258.59</v>
       </c>
       <c r="C219">
-        <v>8711</v>
+        <v>28444</v>
       </c>
       <c r="D219">
         <v>0</v>
@@ -4849,10 +4849,10 @@
         <v>223</v>
       </c>
       <c r="B220">
-        <v>129.16</v>
+        <v>1343.46</v>
       </c>
       <c r="C220">
-        <v>8893</v>
+        <v>28078</v>
       </c>
       <c r="D220">
         <v>0</v>
@@ -4866,16 +4866,16 @@
         <v>224</v>
       </c>
       <c r="B221">
-        <v>53127.40000000001</v>
+        <v>282036.14</v>
       </c>
       <c r="C221">
-        <v>1149629</v>
+        <v>6292738</v>
       </c>
       <c r="D221">
-        <v>2000.01</v>
+        <v>9427.330000000002</v>
       </c>
       <c r="E221">
-        <v>219</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -4913,16 +4913,16 @@
         <v>226</v>
       </c>
       <c r="B2">
-        <v>10656.66</v>
+        <v>50004.78</v>
       </c>
       <c r="C2">
-        <v>236068</v>
+        <v>1199285</v>
       </c>
       <c r="D2">
-        <v>390.11</v>
+        <v>2060.320000000001</v>
       </c>
       <c r="E2">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4930,16 +4930,16 @@
         <v>227</v>
       </c>
       <c r="B3">
-        <v>9706.710000000001</v>
+        <v>50238.09999999998</v>
       </c>
       <c r="C3">
-        <v>227603</v>
+        <v>1165795</v>
       </c>
       <c r="D3">
-        <v>633.78</v>
+        <v>2943.79</v>
       </c>
       <c r="E3">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4947,16 +4947,16 @@
         <v>228</v>
       </c>
       <c r="B4">
-        <v>11757.64</v>
+        <v>62882.11999999997</v>
       </c>
       <c r="C4">
-        <v>209584</v>
+        <v>1235319</v>
       </c>
       <c r="D4">
-        <v>515.16</v>
+        <v>1856.34</v>
       </c>
       <c r="E4">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4964,16 +4964,16 @@
         <v>229</v>
       </c>
       <c r="B5">
-        <v>10822.82</v>
+        <v>57767.32000000001</v>
       </c>
       <c r="C5">
-        <v>226327</v>
+        <v>1255024</v>
       </c>
       <c r="D5">
-        <v>187.21</v>
+        <v>1253.59</v>
       </c>
       <c r="E5">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4981,16 +4981,16 @@
         <v>230</v>
       </c>
       <c r="B6">
-        <v>10183.57</v>
+        <v>61143.81999999999</v>
       </c>
       <c r="C6">
-        <v>250047</v>
+        <v>1437315</v>
       </c>
       <c r="D6">
-        <v>273.7500000000001</v>
+        <v>1313.29</v>
       </c>
       <c r="E6">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -4998,16 +4998,16 @@
         <v>224</v>
       </c>
       <c r="B7">
-        <v>53127.40000000001</v>
+        <v>282036.14</v>
       </c>
       <c r="C7">
-        <v>1149629</v>
+        <v>6292738</v>
       </c>
       <c r="D7">
-        <v>2000.01</v>
+        <v>9427.33</v>
       </c>
       <c r="E7">
-        <v>219</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -5045,16 +5045,16 @@
         <v>232</v>
       </c>
       <c r="B2">
-        <v>11154.43</v>
+        <v>61935.96999999996</v>
       </c>
       <c r="C2">
-        <v>231079</v>
+        <v>1421439</v>
       </c>
       <c r="D2">
-        <v>442.42</v>
+        <v>1425.85</v>
       </c>
       <c r="E2">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5062,16 +5062,16 @@
         <v>233</v>
       </c>
       <c r="B3">
-        <v>9860.74</v>
+        <v>52264.16000000001</v>
       </c>
       <c r="C3">
-        <v>211382</v>
+        <v>1176901</v>
       </c>
       <c r="D3">
-        <v>522.58</v>
+        <v>2495.12</v>
       </c>
       <c r="E3">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5079,16 +5079,16 @@
         <v>234</v>
       </c>
       <c r="B4">
-        <v>11365.56</v>
+        <v>58027.18</v>
       </c>
       <c r="C4">
-        <v>250605</v>
+        <v>1285864</v>
       </c>
       <c r="D4">
-        <v>628.73</v>
+        <v>3165.269999999999</v>
       </c>
       <c r="E4">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5096,16 +5096,16 @@
         <v>235</v>
       </c>
       <c r="B5">
-        <v>9467.750000000002</v>
+        <v>56786.54999999998</v>
       </c>
       <c r="C5">
-        <v>207078</v>
+        <v>1281556</v>
       </c>
       <c r="D5">
-        <v>272.53</v>
+        <v>1623.17</v>
       </c>
       <c r="E5">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5113,16 +5113,16 @@
         <v>236</v>
       </c>
       <c r="B6">
-        <v>11278.92</v>
+        <v>53022.28000000002</v>
       </c>
       <c r="C6">
-        <v>249485</v>
+        <v>1126978</v>
       </c>
       <c r="D6">
-        <v>133.75</v>
+        <v>717.9200000000001</v>
       </c>
       <c r="E6">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5130,16 +5130,16 @@
         <v>224</v>
       </c>
       <c r="B7">
-        <v>53127.39999999999</v>
+        <v>282036.14</v>
       </c>
       <c r="C7">
-        <v>1149629</v>
+        <v>6292738</v>
       </c>
       <c r="D7">
-        <v>2000.01</v>
+        <v>9427.33</v>
       </c>
       <c r="E7">
-        <v>219</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -5177,13 +5177,13 @@
         <v>238</v>
       </c>
       <c r="B2">
-        <v>6174.3</v>
+        <v>22850.44</v>
       </c>
       <c r="C2">
-        <v>130299</v>
+        <v>550709</v>
       </c>
       <c r="D2">
-        <v>352.04</v>
+        <v>1477.54</v>
       </c>
       <c r="E2">
         <v>24</v>
@@ -5194,13 +5194,13 @@
         <v>239</v>
       </c>
       <c r="B3">
-        <v>3604.27</v>
+        <v>23354.83000000001</v>
       </c>
       <c r="C3">
-        <v>122241</v>
+        <v>558939</v>
       </c>
       <c r="D3">
-        <v>17.14</v>
+        <v>124.78</v>
       </c>
       <c r="E3">
         <v>24</v>
@@ -5211,13 +5211,13 @@
         <v>240</v>
       </c>
       <c r="B4">
-        <v>5456.91</v>
+        <v>21258.3</v>
       </c>
       <c r="C4">
-        <v>127058</v>
+        <v>520761</v>
       </c>
       <c r="D4">
-        <v>51.24000000000001</v>
+        <v>277.1300000000001</v>
       </c>
       <c r="E4">
         <v>25</v>
@@ -5228,13 +5228,13 @@
         <v>241</v>
       </c>
       <c r="B5">
-        <v>8888.600000000002</v>
+        <v>26702.21</v>
       </c>
       <c r="C5">
-        <v>132452</v>
+        <v>497795</v>
       </c>
       <c r="D5">
-        <v>506.5599999999999</v>
+        <v>1480.82</v>
       </c>
       <c r="E5">
         <v>25</v>
@@ -5245,13 +5245,13 @@
         <v>242</v>
       </c>
       <c r="B6">
-        <v>5226.15</v>
+        <v>23663.52</v>
       </c>
       <c r="C6">
-        <v>114779</v>
+        <v>540889</v>
       </c>
       <c r="D6">
-        <v>104.28</v>
+        <v>314.59</v>
       </c>
       <c r="E6">
         <v>24</v>
@@ -5262,13 +5262,13 @@
         <v>243</v>
       </c>
       <c r="B7">
-        <v>4797.839999999999</v>
+        <v>23299.85</v>
       </c>
       <c r="C7">
-        <v>131721</v>
+        <v>567217</v>
       </c>
       <c r="D7">
-        <v>71.48</v>
+        <v>468.17</v>
       </c>
       <c r="E7">
         <v>25</v>
@@ -5279,13 +5279,13 @@
         <v>244</v>
       </c>
       <c r="B8">
-        <v>7658.099999999999</v>
+        <v>23106.33</v>
       </c>
       <c r="C8">
-        <v>128145</v>
+        <v>471673</v>
       </c>
       <c r="D8">
-        <v>333.39</v>
+        <v>711.6299999999999</v>
       </c>
       <c r="E8">
         <v>24</v>
@@ -5296,13 +5296,13 @@
         <v>245</v>
       </c>
       <c r="B9">
-        <v>5039.79</v>
+        <v>25155.41000000001</v>
       </c>
       <c r="C9">
-        <v>126442</v>
+        <v>637554</v>
       </c>
       <c r="D9">
-        <v>139.91</v>
+        <v>632.96</v>
       </c>
       <c r="E9">
         <v>23</v>
@@ -5313,16 +5313,16 @@
         <v>246</v>
       </c>
       <c r="B10">
-        <v>6281.439999999999</v>
+        <v>92645.24999999993</v>
       </c>
       <c r="C10">
-        <v>136492</v>
+        <v>1947201</v>
       </c>
       <c r="D10">
-        <v>423.97</v>
+        <v>3939.71</v>
       </c>
       <c r="E10">
-        <v>25</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5330,16 +5330,16 @@
         <v>224</v>
       </c>
       <c r="B11">
-        <v>53127.39999999999</v>
+        <v>282036.1399999999</v>
       </c>
       <c r="C11">
-        <v>1149629</v>
+        <v>6292738</v>
       </c>
       <c r="D11">
-        <v>2000.01</v>
+        <v>9427.330000000002</v>
       </c>
       <c r="E11">
-        <v>219</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Fix 'Count' column creatation
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1152,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1186,7 +1186,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1203,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1237,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1254,7 +1254,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1271,7 +1271,7 @@
         <v>86.86999999999999</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1288,7 +1288,7 @@
         <v>53.87</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1305,7 +1305,7 @@
         <v>0</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1339,7 +1339,7 @@
         <v>39.63999999999999</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1373,7 +1373,7 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1390,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1407,7 +1407,7 @@
         <v>133.7</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1424,7 +1424,7 @@
         <v>111.81</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1458,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1475,7 +1475,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1492,7 +1492,7 @@
         <v>171.38</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1509,7 +1509,7 @@
         <v>0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1526,7 +1526,7 @@
         <v>216.69</v>
       </c>
       <c r="E24">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1543,7 +1543,7 @@
         <v>98.00000000000003</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1560,7 +1560,7 @@
         <v>760.4</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1662,7 +1662,7 @@
         <v>190.45</v>
       </c>
       <c r="E32">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1679,7 +1679,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1696,7 +1696,7 @@
         <v>42.28</v>
       </c>
       <c r="E34">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1713,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="E35">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1730,7 +1730,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1747,7 +1747,7 @@
         <v>0</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1764,7 +1764,7 @@
         <v>5.7</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1798,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="E40">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1815,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1849,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1866,7 +1866,7 @@
         <v>149.53</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1883,7 +1883,7 @@
         <v>343.74</v>
       </c>
       <c r="E45">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1900,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1917,7 +1917,7 @@
         <v>0</v>
       </c>
       <c r="E47">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1934,7 +1934,7 @@
         <v>108.17</v>
       </c>
       <c r="E48">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1951,7 +1951,7 @@
         <v>0</v>
       </c>
       <c r="E49">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1968,7 +1968,7 @@
         <v>0</v>
       </c>
       <c r="E50">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1985,7 +1985,7 @@
         <v>13.9</v>
       </c>
       <c r="E51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="E52">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2019,7 +2019,7 @@
         <v>0</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2036,7 +2036,7 @@
         <v>78.09999999999999</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2053,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2070,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="E56">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2087,7 +2087,7 @@
         <v>0</v>
       </c>
       <c r="E57">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2104,7 +2104,7 @@
         <v>56.89</v>
       </c>
       <c r="E58">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2138,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="E60">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2155,7 +2155,7 @@
         <v>0</v>
       </c>
       <c r="E61">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2172,7 +2172,7 @@
         <v>488.34</v>
       </c>
       <c r="E62">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2189,7 +2189,7 @@
         <v>0</v>
       </c>
       <c r="E63">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2206,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="E64">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2240,7 +2240,7 @@
         <v>229.77</v>
       </c>
       <c r="E66">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2257,7 +2257,7 @@
         <v>0</v>
       </c>
       <c r="E67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2274,7 +2274,7 @@
         <v>166.98</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2291,7 +2291,7 @@
         <v>0</v>
       </c>
       <c r="E69">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2308,7 +2308,7 @@
         <v>37.88</v>
       </c>
       <c r="E70">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2325,7 +2325,7 @@
         <v>487.95</v>
       </c>
       <c r="E71">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2342,7 +2342,7 @@
         <v>637.11</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2359,7 +2359,7 @@
         <v>0</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2376,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="E75">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2410,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="E76">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2427,7 +2427,7 @@
         <v>111.83</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2444,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="E78">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2461,7 +2461,7 @@
         <v>72.14</v>
       </c>
       <c r="E79">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2478,7 +2478,7 @@
         <v>92.75</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2529,7 +2529,7 @@
         <v>0</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2546,7 +2546,7 @@
         <v>0</v>
       </c>
       <c r="E84">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2580,7 +2580,7 @@
         <v>18.24</v>
       </c>
       <c r="E86">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2597,7 +2597,7 @@
         <v>0</v>
       </c>
       <c r="E87">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2614,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="E88">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2631,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2648,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2665,7 +2665,7 @@
         <v>0</v>
       </c>
       <c r="E91">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2682,7 +2682,7 @@
         <v>325.58</v>
       </c>
       <c r="E92">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2699,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2716,7 +2716,7 @@
         <v>0</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2750,7 +2750,7 @@
         <v>0</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2767,7 +2767,7 @@
         <v>0</v>
       </c>
       <c r="E97">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2784,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="E98">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2801,7 +2801,7 @@
         <v>69.20999999999999</v>
       </c>
       <c r="E99">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2818,7 +2818,7 @@
         <v>0</v>
       </c>
       <c r="E100">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2835,7 +2835,7 @@
         <v>705.97</v>
       </c>
       <c r="E101">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2852,7 +2852,7 @@
         <v>40.17</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2869,7 +2869,7 @@
         <v>0</v>
       </c>
       <c r="E103">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2886,7 +2886,7 @@
         <v>0</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2903,7 +2903,7 @@
         <v>280.05</v>
       </c>
       <c r="E105">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2920,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="E106">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2937,7 +2937,7 @@
         <v>0</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2954,7 +2954,7 @@
         <v>0</v>
       </c>
       <c r="E108">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2971,7 +2971,7 @@
         <v>0</v>
       </c>
       <c r="E109">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2988,7 +2988,7 @@
         <v>46.15</v>
       </c>
       <c r="E110">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -3005,7 +3005,7 @@
         <v>0</v>
       </c>
       <c r="E111">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -3039,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="E113">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -3056,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="E114">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -3073,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="E115">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -3090,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="E116">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -3107,7 +3107,7 @@
         <v>203.34</v>
       </c>
       <c r="E117">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -3124,7 +3124,7 @@
         <v>0</v>
       </c>
       <c r="E118">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3141,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="E119">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3158,7 +3158,7 @@
         <v>23.9</v>
       </c>
       <c r="E120">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -3175,7 +3175,7 @@
         <v>0</v>
       </c>
       <c r="E121">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3192,7 +3192,7 @@
         <v>105.19</v>
       </c>
       <c r="E122">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3209,7 +3209,7 @@
         <v>0</v>
       </c>
       <c r="E123">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3226,7 +3226,7 @@
         <v>0</v>
       </c>
       <c r="E124">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -3243,7 +3243,7 @@
         <v>0</v>
       </c>
       <c r="E125">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -3277,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="E127">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3294,7 +3294,7 @@
         <v>10.11</v>
       </c>
       <c r="E128">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3311,7 +3311,7 @@
         <v>0</v>
       </c>
       <c r="E129">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3328,7 +3328,7 @@
         <v>0</v>
       </c>
       <c r="E130">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3345,7 +3345,7 @@
         <v>0</v>
       </c>
       <c r="E131">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3362,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="E132">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3379,7 +3379,7 @@
         <v>0</v>
       </c>
       <c r="E133">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3413,7 +3413,7 @@
         <v>0</v>
       </c>
       <c r="E135">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3430,7 +3430,7 @@
         <v>0</v>
       </c>
       <c r="E136">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="E137">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3464,7 +3464,7 @@
         <v>0</v>
       </c>
       <c r="E138">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3481,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="E139">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3498,7 +3498,7 @@
         <v>306.22</v>
       </c>
       <c r="E140">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3515,7 +3515,7 @@
         <v>0</v>
       </c>
       <c r="E141">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3532,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="E142">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -3549,7 +3549,7 @@
         <v>0</v>
       </c>
       <c r="E143">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3566,7 +3566,7 @@
         <v>0</v>
       </c>
       <c r="E144">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3583,7 +3583,7 @@
         <v>0</v>
       </c>
       <c r="E145">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3617,7 +3617,7 @@
         <v>0</v>
       </c>
       <c r="E147">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3634,7 +3634,7 @@
         <v>41.05</v>
       </c>
       <c r="E148">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3651,7 +3651,7 @@
         <v>0</v>
       </c>
       <c r="E149">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3668,7 +3668,7 @@
         <v>0</v>
       </c>
       <c r="E150">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -3685,7 +3685,7 @@
         <v>0</v>
       </c>
       <c r="E151">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -3702,7 +3702,7 @@
         <v>0</v>
       </c>
       <c r="E152">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3736,7 +3736,7 @@
         <v>0</v>
       </c>
       <c r="E154">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -3753,7 +3753,7 @@
         <v>0</v>
       </c>
       <c r="E155">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3770,7 +3770,7 @@
         <v>0</v>
       </c>
       <c r="E156">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -3787,7 +3787,7 @@
         <v>0</v>
       </c>
       <c r="E157">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -3804,7 +3804,7 @@
         <v>386.04</v>
       </c>
       <c r="E158">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -3821,7 +3821,7 @@
         <v>0</v>
       </c>
       <c r="E159">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -3855,7 +3855,7 @@
         <v>68.09</v>
       </c>
       <c r="E161">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -3872,7 +3872,7 @@
         <v>0</v>
       </c>
       <c r="E162">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -3889,7 +3889,7 @@
         <v>0</v>
       </c>
       <c r="E163">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -3906,7 +3906,7 @@
         <v>74.72999999999999</v>
       </c>
       <c r="E164">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -3923,7 +3923,7 @@
         <v>0</v>
       </c>
       <c r="E165">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -3940,7 +3940,7 @@
         <v>0</v>
       </c>
       <c r="E166">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -3957,7 +3957,7 @@
         <v>0</v>
       </c>
       <c r="E167">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -3974,7 +3974,7 @@
         <v>5.59</v>
       </c>
       <c r="E168">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169" spans="1:5">
@@ -3991,7 +3991,7 @@
         <v>0</v>
       </c>
       <c r="E169">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="170" spans="1:5">
@@ -4008,7 +4008,7 @@
         <v>0</v>
       </c>
       <c r="E170">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -4025,7 +4025,7 @@
         <v>0</v>
       </c>
       <c r="E171">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -4042,7 +4042,7 @@
         <v>0</v>
       </c>
       <c r="E172">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -4059,7 +4059,7 @@
         <v>0</v>
       </c>
       <c r="E173">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174" spans="1:5">
@@ -4093,7 +4093,7 @@
         <v>298.18</v>
       </c>
       <c r="E175">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4110,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="E176">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -4144,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="E178">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -4161,7 +4161,7 @@
         <v>0</v>
       </c>
       <c r="E179">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:5">
@@ -4178,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="E180">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -4195,7 +4195,7 @@
         <v>0</v>
       </c>
       <c r="E181">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -4212,7 +4212,7 @@
         <v>0</v>
       </c>
       <c r="E182">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -4229,7 +4229,7 @@
         <v>0</v>
       </c>
       <c r="E183">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -4246,7 +4246,7 @@
         <v>241.37</v>
       </c>
       <c r="E184">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -4263,7 +4263,7 @@
         <v>230.18</v>
       </c>
       <c r="E185">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -4280,7 +4280,7 @@
         <v>55.57</v>
       </c>
       <c r="E186">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -4297,7 +4297,7 @@
         <v>0</v>
       </c>
       <c r="E187">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -4314,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="E188">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -4348,7 +4348,7 @@
         <v>0</v>
       </c>
       <c r="E190">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -4365,7 +4365,7 @@
         <v>108.57</v>
       </c>
       <c r="E191">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4382,7 +4382,7 @@
         <v>0</v>
       </c>
       <c r="E192">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -4399,7 +4399,7 @@
         <v>0</v>
       </c>
       <c r="E193">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -4416,7 +4416,7 @@
         <v>0</v>
       </c>
       <c r="E194">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -4433,7 +4433,7 @@
         <v>0</v>
       </c>
       <c r="E195">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -4450,7 +4450,7 @@
         <v>0</v>
       </c>
       <c r="E196">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -4467,7 +4467,7 @@
         <v>0</v>
       </c>
       <c r="E197">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4484,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="E198">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -4501,7 +4501,7 @@
         <v>0</v>
       </c>
       <c r="E199">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4518,7 +4518,7 @@
         <v>0</v>
       </c>
       <c r="E200">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -4535,7 +4535,7 @@
         <v>0</v>
       </c>
       <c r="E201">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4552,7 +4552,7 @@
         <v>445.67</v>
       </c>
       <c r="E202">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4569,7 +4569,7 @@
         <v>0</v>
       </c>
       <c r="E203">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4586,7 +4586,7 @@
         <v>0</v>
       </c>
       <c r="E204">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4603,7 +4603,7 @@
         <v>0</v>
       </c>
       <c r="E205">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4620,7 +4620,7 @@
         <v>0</v>
       </c>
       <c r="E206">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -4637,7 +4637,7 @@
         <v>0</v>
       </c>
       <c r="E207">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -4654,7 +4654,7 @@
         <v>0</v>
       </c>
       <c r="E208">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -4671,7 +4671,7 @@
         <v>94.11</v>
       </c>
       <c r="E209">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -4688,7 +4688,7 @@
         <v>0</v>
       </c>
       <c r="E210">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -4705,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="E211">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -4722,7 +4722,7 @@
         <v>36.2</v>
       </c>
       <c r="E212">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -4739,7 +4739,7 @@
         <v>0</v>
       </c>
       <c r="E213">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -4756,7 +4756,7 @@
         <v>0</v>
       </c>
       <c r="E214">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -4773,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="E215">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -4790,7 +4790,7 @@
         <v>0</v>
       </c>
       <c r="E216">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -4807,7 +4807,7 @@
         <v>0</v>
       </c>
       <c r="E217">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -4824,7 +4824,7 @@
         <v>101.62</v>
       </c>
       <c r="E218">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -4841,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="E219">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -4858,7 +4858,7 @@
         <v>0</v>
       </c>
       <c r="E220">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -4875,7 +4875,7 @@
         <v>9427.330000000002</v>
       </c>
       <c r="E221">
-        <v>242</v>
+        <v>1176</v>
       </c>
     </row>
   </sheetData>
@@ -4922,7 +4922,7 @@
         <v>2060.320000000001</v>
       </c>
       <c r="E2">
-        <v>47</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4939,7 +4939,7 @@
         <v>2943.79</v>
       </c>
       <c r="E3">
-        <v>49</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -4956,7 +4956,7 @@
         <v>1856.34</v>
       </c>
       <c r="E4">
-        <v>48</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -4973,7 +4973,7 @@
         <v>1253.59</v>
       </c>
       <c r="E5">
-        <v>49</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -4990,7 +4990,7 @@
         <v>1313.29</v>
       </c>
       <c r="E6">
-        <v>49</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5007,7 +5007,7 @@
         <v>9427.33</v>
       </c>
       <c r="E7">
-        <v>242</v>
+        <v>1176</v>
       </c>
     </row>
   </sheetData>
@@ -5054,7 +5054,7 @@
         <v>1425.85</v>
       </c>
       <c r="E2">
-        <v>49</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5071,7 +5071,7 @@
         <v>2495.12</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5088,7 +5088,7 @@
         <v>3165.269999999999</v>
       </c>
       <c r="E4">
-        <v>48</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5105,7 +5105,7 @@
         <v>1623.17</v>
       </c>
       <c r="E5">
-        <v>48</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5122,7 +5122,7 @@
         <v>717.9200000000001</v>
       </c>
       <c r="E6">
-        <v>47</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5139,7 +5139,7 @@
         <v>9427.33</v>
       </c>
       <c r="E7">
-        <v>242</v>
+        <v>1176</v>
       </c>
     </row>
   </sheetData>
@@ -5186,7 +5186,7 @@
         <v>1477.54</v>
       </c>
       <c r="E2">
-        <v>24</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -5203,7 +5203,7 @@
         <v>124.78</v>
       </c>
       <c r="E3">
-        <v>24</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -5220,7 +5220,7 @@
         <v>277.1300000000001</v>
       </c>
       <c r="E4">
-        <v>25</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -5237,7 +5237,7 @@
         <v>1480.82</v>
       </c>
       <c r="E5">
-        <v>25</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -5254,7 +5254,7 @@
         <v>314.59</v>
       </c>
       <c r="E6">
-        <v>24</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -5271,7 +5271,7 @@
         <v>468.17</v>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -5288,7 +5288,7 @@
         <v>711.6299999999999</v>
       </c>
       <c r="E8">
-        <v>24</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -5305,7 +5305,7 @@
         <v>632.96</v>
       </c>
       <c r="E9">
-        <v>23</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -5322,7 +5322,7 @@
         <v>3939.71</v>
       </c>
       <c r="E10">
-        <v>48</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -5339,7 +5339,7 @@
         <v>9427.330000000002</v>
       </c>
       <c r="E11">
-        <v>242</v>
+        <v>1176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>